<commit_message>
add log to file
Signed-off-by: ieb <ieb@wevioo.com>
</commit_message>
<xml_diff>
--- a/tnr-auto/DocTest1.xlsx
+++ b/tnr-auto/DocTest1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tiers" sheetId="1" state="visible" r:id="rId2"/>
@@ -242,6 +242,33 @@
     <t xml:space="preserve">02/12/1967</t>
   </si>
   <si>
+    <t xml:space="preserve">555167182</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test resiliation 555167182</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test resiliation 555167183</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test resiliation 555167184</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test resiliation 555167185</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Résiliation aliénation du bien</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Résiliation décès Ass immédiat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Résiliation pour impayé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Résiliation échéance compagnie</t>
+  </si>
+  <si>
     <t xml:space="preserve">Contrat</t>
   </si>
   <si>
@@ -251,9 +278,6 @@
     <t xml:space="preserve">501734539</t>
   </si>
   <si>
-    <t xml:space="preserve">Résiliation échéance compagnie</t>
-  </si>
-  <si>
     <t xml:space="preserve">501848788</t>
   </si>
   <si>
@@ -285,30 +309,6 @@
   </si>
   <si>
     <t xml:space="preserve">501760546</t>
-  </si>
-  <si>
-    <t xml:space="preserve">555167182</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test resiliation 555167182</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test resiliation 555167183</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test resiliation 555167184</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test resiliation 555167185</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Résiliation aliénation du bien</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Résiliation décès Ass immédiat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Résiliation pour impayé</t>
   </si>
   <si>
     <t xml:space="preserve">Sinistre</t>
@@ -426,16 +426,16 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color rgb="FF5C5C5C"/>
       <name val="Tahoma"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -475,14 +475,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFBFBFBF"/>
+        <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFBFBFBF"/>
-        <bgColor rgb="FFCCCCFF"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -555,23 +555,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -587,23 +587,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -687,7 +687,7 @@
   <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N3" activeCellId="1" sqref="B2:B13 N3"/>
+      <selection pane="topLeft" activeCell="N3" activeCellId="1" sqref="A29:G49 N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -973,10 +973,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S24"/>
+  <dimension ref="A1:S45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="1" sqref="B2:B13 A19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29:G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1866,6 +1866,207 @@
         <v>99201354</v>
       </c>
     </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4"/>
+      <c r="B29" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4"/>
+      <c r="B30" s="5" t="n">
+        <v>555230879</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="4"/>
+      <c r="B31" s="5" t="n">
+        <v>555166789</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="4"/>
+      <c r="B32" s="5" t="n">
+        <v>555151191</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="4"/>
+      <c r="B35" s="5" t="n">
+        <v>555167182</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="4"/>
+      <c r="B36" s="5" t="n">
+        <v>555230879</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="4"/>
+      <c r="B37" s="5" t="n">
+        <v>555166789</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="4"/>
+      <c r="B38" s="5" t="n">
+        <v>555151191</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="4"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="4"/>
+      <c r="B40" s="6" t="n">
+        <v>555077287</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="4"/>
+      <c r="B41" s="6" t="n">
+        <v>555070126</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="4"/>
+      <c r="B42" s="6" t="n">
+        <v>555237532</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="4"/>
+      <c r="B43" s="6" t="n">
+        <v>555236169</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="4"/>
+      <c r="B44" s="6" t="n">
+        <v>555067110</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1882,10 +2083,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:B13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="A29:G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1900,58 +2101,58 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>74</v>
+      <c r="A2" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>74</v>
+      <c r="A3" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>74</v>
+      <c r="A4" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>74</v>
+      <c r="A5" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>74</v>
+      <c r="A6" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>79</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>74</v>
       </c>
       <c r="E7" s="0"/>
       <c r="F7" s="0"/>
@@ -1959,11 +2160,11 @@
       <c r="H7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>74</v>
+      <c r="A8" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>79</v>
       </c>
       <c r="E8" s="0"/>
       <c r="F8" s="0"/>
@@ -1971,11 +2172,11 @@
       <c r="H8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>74</v>
+      <c r="A9" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>79</v>
       </c>
       <c r="E9" s="0"/>
       <c r="F9" s="0"/>
@@ -1983,11 +2184,11 @@
       <c r="H9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>74</v>
+      <c r="A10" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>79</v>
       </c>
       <c r="E10" s="0"/>
       <c r="F10" s="0"/>
@@ -1995,11 +2196,11 @@
       <c r="H10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>74</v>
+      <c r="A11" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>79</v>
       </c>
       <c r="E11" s="0"/>
       <c r="F11" s="0"/>
@@ -2007,11 +2208,11 @@
       <c r="H11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>74</v>
+      <c r="A12" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>79</v>
       </c>
       <c r="E12" s="0"/>
       <c r="F12" s="0"/>
@@ -2019,167 +2220,43 @@
       <c r="H12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>74</v>
+      <c r="A13" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>79</v>
       </c>
       <c r="E13" s="0"/>
       <c r="F13" s="0"/>
       <c r="G13" s="0"/>
       <c r="H13" s="0"/>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0"/>
-      <c r="B14" s="0"/>
-      <c r="E14" s="0"/>
-      <c r="F14" s="0"/>
-      <c r="G14" s="0"/>
-      <c r="H14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0"/>
-      <c r="B15" s="0"/>
-      <c r="E15" s="0"/>
-      <c r="F15" s="0"/>
-      <c r="G15" s="0"/>
-      <c r="H15" s="0"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0"/>
-      <c r="B16" s="0"/>
-      <c r="E16" s="0"/>
-      <c r="F16" s="0"/>
-      <c r="G16" s="0"/>
-      <c r="H16" s="0"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0"/>
-      <c r="B17" s="0"/>
-      <c r="E17" s="0"/>
-      <c r="F17" s="0"/>
-      <c r="G17" s="0"/>
-      <c r="H17" s="0"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0"/>
-      <c r="B18" s="0"/>
-      <c r="E18" s="0"/>
-      <c r="F18" s="0"/>
-      <c r="G18" s="0"/>
-      <c r="H18" s="0"/>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E30" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E31" s="7" t="n">
-        <v>555230879</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E32" s="7" t="n">
-        <v>555166789</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E33" s="7" t="n">
-        <v>555151191</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E36" s="7" t="n">
-        <v>555167182</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E37" s="7" t="n">
-        <v>555230879</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E38" s="7" t="n">
-        <v>555166789</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E39" s="7" t="n">
-        <v>555151191</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E40" s="7"/>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E41" s="8" t="n">
-        <v>555077287</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E42" s="8" t="n">
-        <v>555070126</v>
-      </c>
-      <c r="F42" s="9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E43" s="8" t="n">
-        <v>555237532</v>
-      </c>
-      <c r="F43" s="9" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E44" s="8" t="n">
-        <v>555236169</v>
-      </c>
-      <c r="F44" s="9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E45" s="8" t="n">
-        <v>555067110</v>
-      </c>
-      <c r="F45" s="9" t="s">
-        <v>74</v>
-      </c>
-    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2199,7 +2276,7 @@
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="B2:B13 C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="A29:G49 C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2330,7 +2407,7 @@
       <c r="A15" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="7" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2338,7 +2415,7 @@
       <c r="A16" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="7" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2346,7 +2423,7 @@
       <c r="A17" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="7" t="s">
         <v>109</v>
       </c>
     </row>
@@ -2354,7 +2431,7 @@
       <c r="A18" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="7" t="s">
         <v>115</v>
       </c>
     </row>
@@ -2362,7 +2439,7 @@
       <c r="A19" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="7" t="s">
         <v>109</v>
       </c>
     </row>
@@ -2452,7 +2529,7 @@
   <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F20" activeCellId="1" sqref="B2:B13 F20"/>
+      <selection pane="topLeft" activeCell="F20" activeCellId="1" sqref="A29:G49 F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>